<commit_message>
Author : Ruchit Jain Description: Updated Training_Partner.xlsx              Added batchtype column
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Training_Partner.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Training_Partner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>trainingPartnerName</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Any</t>
+  </si>
+  <si>
+    <t>batchType</t>
+  </si>
+  <si>
+    <t>PMKVY/NON-PMKVY</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -161,6 +167,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -465,21 +474,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.21875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="51.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -489,8 +499,11 @@
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -499,6 +512,9 @@
       </c>
       <c r="C2" s="7" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Author : Ruchit Jain Description : Updated TP excel sheet
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Training_Partner.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Training_Partner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>trainingPartnerName</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>Any</t>
-  </si>
-  <si>
-    <t>batchType</t>
-  </si>
-  <si>
-    <t>PMKVY/NON-PMKVY</t>
   </si>
 </sst>
 </file>
@@ -141,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -167,9 +161,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,22 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="51.21875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -499,11 +489,8 @@
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -512,9 +499,6 @@
       </c>
       <c r="C2" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>